<commit_message>
Update 2016 CrystalDiskMark Result Comparisons.xlsx
</commit_message>
<xml_diff>
--- a/benchmarking/CrystalDiskMark (Disk Read-Write Speeds)/_Results/2016 CrystalDiskMark Result Comparisons.xlsx
+++ b/benchmarking/CrystalDiskMark (Disk Read-Write Speeds)/_Results/2016 CrystalDiskMark Result Comparisons.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcavallo\OneDrive\Stuff\Speed Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcava\Documents\GitHub\Coding\benchmarking\CrystalDiskMark (Disk Read-Write Speeds)\_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B246344F-35B6-4CA2-8EFC-4DEE2B6909C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" tabRatio="824" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USB Flash Drives" sheetId="12" r:id="rId1"/>
@@ -22,10 +23,19 @@
     <sheet name="X1 Carbon C" sheetId="10" r:id="rId8"/>
     <sheet name="Intel NUC C" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -223,7 +233,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -587,487 +597,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF21FF46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1829,11 +1359,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q48"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3149,11 +2679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3978,109 +3508,109 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:K14">
-    <cfRule type="top10" dxfId="95" priority="121" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="94" priority="122" rank="1"/>
+    <cfRule type="top10" dxfId="47" priority="121" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="122" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:K11">
-    <cfRule type="top10" dxfId="93" priority="125" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="92" priority="126" rank="1"/>
+    <cfRule type="top10" dxfId="45" priority="125" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="44" priority="126" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:K8">
-    <cfRule type="top10" dxfId="91" priority="129" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="90" priority="130" rank="1"/>
+    <cfRule type="top10" dxfId="43" priority="129" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="42" priority="130" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:K6">
-    <cfRule type="top10" dxfId="89" priority="133" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="88" priority="134" rank="1"/>
+    <cfRule type="top10" dxfId="41" priority="133" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="40" priority="134" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:K16">
-    <cfRule type="top10" dxfId="87" priority="137" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="86" priority="138" rank="1"/>
+    <cfRule type="top10" dxfId="39" priority="137" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="38" priority="138" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:K18">
-    <cfRule type="top10" dxfId="85" priority="141" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="84" priority="142" rank="1"/>
+    <cfRule type="top10" dxfId="37" priority="141" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="36" priority="142" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:K21">
-    <cfRule type="top10" dxfId="83" priority="145" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="82" priority="146" rank="1"/>
+    <cfRule type="top10" dxfId="35" priority="145" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="146" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:K24">
-    <cfRule type="top10" dxfId="81" priority="149" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="80" priority="150" rank="1"/>
+    <cfRule type="top10" dxfId="33" priority="149" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="150" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:K10">
-    <cfRule type="top10" dxfId="79" priority="153" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="78" priority="154" rank="1"/>
+    <cfRule type="top10" dxfId="31" priority="153" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="30" priority="154" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:K13">
-    <cfRule type="top10" dxfId="77" priority="157" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="76" priority="158" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="157" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="158" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:K20">
-    <cfRule type="top10" dxfId="75" priority="161" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="74" priority="162" rank="1"/>
+    <cfRule type="top10" dxfId="27" priority="161" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="162" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:K23">
-    <cfRule type="top10" dxfId="73" priority="165" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="72" priority="166" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="165" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="166" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="top10" dxfId="71" priority="49" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="70" priority="50" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="49" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="50" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="top10" dxfId="69" priority="51" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="68" priority="52" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="51" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="52" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="top10" dxfId="67" priority="53" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="66" priority="54" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="53" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="54" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="top10" dxfId="65" priority="55" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="64" priority="56" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="55" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="56" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="top10" dxfId="63" priority="57" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="62" priority="58" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="57" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="58" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="top10" dxfId="61" priority="59" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="60" priority="60" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="59" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="60" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="top10" dxfId="59" priority="61" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="58" priority="62" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="61" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="62" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="top10" dxfId="57" priority="63" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="56" priority="64" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="63" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="64" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="top10" dxfId="55" priority="65" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="54" priority="66" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="65" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="66" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="top10" dxfId="53" priority="67" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="52" priority="68" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="67" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="68" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="top10" dxfId="51" priority="69" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="50" priority="70" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="69" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="70" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="top10" dxfId="49" priority="71" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="48" priority="72" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="71" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="72" rank="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G4" location="'3570k SSD C'!A1" display="'3570k SSD C'!A1"/>
-    <hyperlink ref="H4" location="'3570k SSD D'!A1" display="'3570k SSD D'!A1"/>
-    <hyperlink ref="I4" location="'3570k HDD E'!A1" display="'3570k HDD E'!A1"/>
-    <hyperlink ref="J4" location="'3570k HDD G'!A1" display="'3570k HDD G'!A1"/>
-    <hyperlink ref="F4" location="'Y50 HDD C'!A1" display="'Y50 HDD C'!A1"/>
-    <hyperlink ref="K4" location="'ONLINE 850 EVO'!A1" display="'ONLINE 850 EVO'!A1"/>
-    <hyperlink ref="L4" location="'ONLINE 850 EVO'!A1" display="'ONLINE 850 EVO'!A1"/>
+    <hyperlink ref="G4" location="'3570k SSD C'!A1" display="'3570k SSD C'!A1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H4" location="'3570k SSD D'!A1" display="'3570k SSD D'!A1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I4" location="'3570k HDD E'!A1" display="'3570k HDD E'!A1" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J4" location="'3570k HDD G'!A1" display="'3570k HDD G'!A1" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="F4" location="'Y50 HDD C'!A1" display="'Y50 HDD C'!A1" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="K4" location="'ONLINE 850 EVO'!A1" display="'ONLINE 850 EVO'!A1" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="L4" location="'ONLINE 850 EVO'!A1" display="'ONLINE 850 EVO'!A1" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4088,7 +3618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4611,7 +4141,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4619,7 +4149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5178,7 +4708,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5186,7 +4716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5695,7 +5225,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5703,7 +5233,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6188,7 +5718,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6196,7 +5726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6681,7 +6211,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6689,11 +6219,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7062,7 +6592,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7070,11 +6600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7443,7 +6973,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Tabulation!A1" display="HOME"/>
+    <hyperlink ref="B2" location="Tabulation!A1" display="HOME" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>